<commit_message>
Update newdir/test.xlsx in en_US
100%  source file: 'newdir/test.xlsx'
on 'en_US'.
</commit_message>
<xml_diff>
--- a/newdir/test.xlsx
+++ b/newdir/test.xlsx
@@ -1,102 +1,61 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
-  <si>
-    <t>en_US</t>
-  </si>
-  <si>
-    <t>context</t>
-  </si>
-  <si>
-    <t>modified</t>
-  </si>
-  <si>
-    <t>fr</t>
-  </si>
-  <si>
-    <t>jp</t>
-  </si>
-  <si>
-    <t>de_DE</t>
-  </si>
-  <si>
-    <t>el</t>
-  </si>
-  <si>
-    <t>fi</t>
-  </si>
-  <si>
-    <t>se</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>example</t>
-  </si>
-  <si>
-    <t>fish</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="10.0"/>
+      <name val="Arial"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="10"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
       <color theme="1"/>
-      <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -294,69 +253,184 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>8</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>en_US</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>context</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>modified</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>fr</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>modified</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>jp</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>modified</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>de_DE</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>el</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>modified</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>fi</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>se</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>es</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>he_IL</t>
+        </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>δοκιμασία</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>2023-11-09</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>examen</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>בדיקה</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>example</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>test 1 fr</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>παράδειγμα</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>2023-11-09</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>ejemplo</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>דוגמא</t>
+        </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>fish</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>test 1 fr</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>ψάρι</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>2023-11-09</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>pez</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>דג</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update newdir/test.xlsx in en_US [Manual Sync]
100% translated source file: 'newdir/test.xlsx'
on 'en_US'.
</commit_message>
<xml_diff>
--- a/newdir/test.xlsx
+++ b/newdir/test.xlsx
@@ -364,7 +364,7 @@
           <t>test</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" s="0" t="inlineStr">
         <is>
           <t>2023-11-09</t>
         </is>
@@ -416,7 +416,7 @@
           <t>test</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
+      <c r="J3" s="0" t="inlineStr">
         <is>
           <t>2023-11-09</t>
         </is>
@@ -468,7 +468,7 @@
           <t>test</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="J4" s="0" t="inlineStr">
         <is>
           <t>2023-11-09</t>
         </is>

</xml_diff>